<commit_message>
#36 Uploading updated UniRentHub documents
</commit_message>
<xml_diff>
--- a/Documents/ProductDocs/4_Testing/Report/C11_TIRT_ver.1.0.xlsx
+++ b/Documents/ProductDocs/4_Testing/Report/C11_TIRT_ver.1.0.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27316"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_98E60DC31B84A44C56753DCC0B97CADE1D96F14E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A04ED767-EBDD-433C-9385-9187F2A84CA3}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="11_98E60DC31B84A44C56753DCC0B97CADE1D96F14E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C22A746C-C6CD-4286-8E7F-D679FD29FF7F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28980" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28980" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="16-01-2024 Esecuzione 1" sheetId="3" r:id="rId1"/>
-    <sheet name="17-01-2024 Esecuzione 2" sheetId="4" r:id="rId2"/>
+    <sheet name="15-01-2024 Esecuzione 1" sheetId="3" r:id="rId1"/>
+    <sheet name="16-01-2024 Esecuzione 2" sheetId="4" r:id="rId2"/>
     <sheet name="Team Members" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="161">
   <si>
     <t>Test Incident Report</t>
   </si>
@@ -46,277 +46,406 @@
     <t>Esecuzione: 1</t>
   </si>
   <si>
+    <t>Data Iterazione: 15/01/2024</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Test Incident ID</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Esito</t>
+  </si>
+  <si>
+    <t>Motivo del Warning</t>
+  </si>
+  <si>
+    <t>Test Passati</t>
+  </si>
+  <si>
+    <t>Test non passati</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>TC_1.1_1</t>
+  </si>
+  <si>
+    <t>TI_1.1_1</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>Not Passed</t>
+  </si>
+  <si>
+    <t>Mancanza alert</t>
+  </si>
+  <si>
+    <t>TC_1.1_2</t>
+  </si>
+  <si>
+    <t>TI_1.1_2</t>
+  </si>
+  <si>
+    <t>TC_1.1_3</t>
+  </si>
+  <si>
+    <t>TI_1.1_3</t>
+  </si>
+  <si>
+    <t>Esecuzione accetta</t>
+  </si>
+  <si>
+    <t>TC_1.1_4</t>
+  </si>
+  <si>
+    <t>TI_1.1_4</t>
+  </si>
+  <si>
+    <t>TC_1.1_5</t>
+  </si>
+  <si>
+    <t>TI_1.1_5</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>TC_2.1_1</t>
+  </si>
+  <si>
+    <t>TI_2.1_1</t>
+  </si>
+  <si>
+    <t>TC_2.1_2</t>
+  </si>
+  <si>
+    <t>TI_2.1_2</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>TC_2.1_3</t>
+  </si>
+  <si>
+    <t>TI_2.1_3</t>
+  </si>
+  <si>
+    <t>TC_2.1_4</t>
+  </si>
+  <si>
+    <t>TI_2.1_4</t>
+  </si>
+  <si>
+    <t>TC_2.1_5</t>
+  </si>
+  <si>
+    <t>TI_2.1_5</t>
+  </si>
+  <si>
+    <t>TC_2.1_6</t>
+  </si>
+  <si>
+    <t>TI_2.1_6</t>
+  </si>
+  <si>
+    <t>TC_2.1_7</t>
+  </si>
+  <si>
+    <t>TI_2.1_7</t>
+  </si>
+  <si>
+    <t>TC_2.1_8</t>
+  </si>
+  <si>
+    <t>TI_2.1_8</t>
+  </si>
+  <si>
+    <t>TC_2.1_9</t>
+  </si>
+  <si>
+    <t>TI_2.1_9</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>TC_2.1_10</t>
+  </si>
+  <si>
+    <t>TI_2.1_10</t>
+  </si>
+  <si>
+    <t>TC_2.1_11</t>
+  </si>
+  <si>
+    <t>TI_2.1_11</t>
+  </si>
+  <si>
+    <t>TC_2.1_12</t>
+  </si>
+  <si>
+    <t>TI_2.1_12</t>
+  </si>
+  <si>
+    <t>TC_2.1_13</t>
+  </si>
+  <si>
+    <t>TI_2.1_13</t>
+  </si>
+  <si>
+    <t>TC_2.1_14</t>
+  </si>
+  <si>
+    <t>TI_2.1_14</t>
+  </si>
+  <si>
+    <t>TC_3.1_1</t>
+  </si>
+  <si>
+    <t>TI_3.1_1</t>
+  </si>
+  <si>
+    <t>TC_3.2_1</t>
+  </si>
+  <si>
+    <t>TI_3.2_1</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>TC_3.2_2</t>
+  </si>
+  <si>
+    <t>TI_3.2_2</t>
+  </si>
+  <si>
+    <t>TC_3.2_3</t>
+  </si>
+  <si>
+    <t>TI_3.2_3</t>
+  </si>
+  <si>
+    <t>TC_3.2_4</t>
+  </si>
+  <si>
+    <t>TI_3.2_4</t>
+  </si>
+  <si>
+    <t>TC_3.2_5</t>
+  </si>
+  <si>
+    <t>TI_3.2_5</t>
+  </si>
+  <si>
+    <t>TC_3.2_6</t>
+  </si>
+  <si>
+    <t>TI_3.2_6</t>
+  </si>
+  <si>
+    <t>TC_3.2_7</t>
+  </si>
+  <si>
+    <t>TI_3.2_7</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>TC_3.3_1</t>
+  </si>
+  <si>
+    <t>TI_3.3_1</t>
+  </si>
+  <si>
+    <t>TC_3.3_2</t>
+  </si>
+  <si>
+    <t>TI_3.3_2</t>
+  </si>
+  <si>
+    <t>TC_3.3_3</t>
+  </si>
+  <si>
+    <t>TI_3.3_3</t>
+  </si>
+  <si>
+    <t>TC_3.3_4</t>
+  </si>
+  <si>
+    <t>TI_3.3_4</t>
+  </si>
+  <si>
+    <t>TC_3.4_1</t>
+  </si>
+  <si>
+    <t>TI_3.4_1</t>
+  </si>
+  <si>
+    <t>TC_3.4_2</t>
+  </si>
+  <si>
+    <t>TI_3.4_2</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>TC_3.4_3</t>
+  </si>
+  <si>
+    <t>TI_3.4_3</t>
+  </si>
+  <si>
+    <t>TC_3.4_4</t>
+  </si>
+  <si>
+    <t>TI_3.4_4</t>
+  </si>
+  <si>
+    <t>TC_3.4_5</t>
+  </si>
+  <si>
+    <t>TI_3.4_5</t>
+  </si>
+  <si>
+    <t>TC_1.1.1</t>
+  </si>
+  <si>
+    <t>TI_1.1.1</t>
+  </si>
+  <si>
+    <t>TC_1.1.2</t>
+  </si>
+  <si>
+    <t>TI_1.1.2</t>
+  </si>
+  <si>
+    <t>Non veniva lanciata l'eccezione</t>
+  </si>
+  <si>
+    <t>TC_1.1.3</t>
+  </si>
+  <si>
+    <t>TI_1.1.3</t>
+  </si>
+  <si>
+    <t>TC_1.1.4</t>
+  </si>
+  <si>
+    <t>TI_1.1.4</t>
+  </si>
+  <si>
+    <t>TC_1.2.1</t>
+  </si>
+  <si>
+    <t>TI_1.2.1</t>
+  </si>
+  <si>
+    <t>TC_1.2.2</t>
+  </si>
+  <si>
+    <t>TI_1.2.2</t>
+  </si>
+  <si>
+    <t>TC_1.2.3</t>
+  </si>
+  <si>
+    <t>TI_1.2.3</t>
+  </si>
+  <si>
+    <t>TC_1.2.4</t>
+  </si>
+  <si>
+    <t>TI_1.2.4</t>
+  </si>
+  <si>
+    <t>TC_2.1.1</t>
+  </si>
+  <si>
+    <t>TI_2.1.1</t>
+  </si>
+  <si>
+    <t>TC_2.1.2</t>
+  </si>
+  <si>
+    <t>TI_2.1.2</t>
+  </si>
+  <si>
+    <t>TC_2.1.3</t>
+  </si>
+  <si>
+    <t>TI_2.1.3</t>
+  </si>
+  <si>
+    <t>TC_2.2.1</t>
+  </si>
+  <si>
+    <t>TI_2.2.1</t>
+  </si>
+  <si>
+    <t>TC_2.2.2</t>
+  </si>
+  <si>
+    <t>TI_2.2.2</t>
+  </si>
+  <si>
+    <t>TC_2.2.3</t>
+  </si>
+  <si>
+    <t>TI_2.2.3</t>
+  </si>
+  <si>
+    <t>TC_3.1.1</t>
+  </si>
+  <si>
+    <t>TI_3.1.1</t>
+  </si>
+  <si>
+    <t>TC_3.1.2</t>
+  </si>
+  <si>
+    <t>TI_3.1.2</t>
+  </si>
+  <si>
+    <t>TC_3.1.3</t>
+  </si>
+  <si>
+    <t>TI_3.1.3</t>
+  </si>
+  <si>
+    <t>TC_3.2.1</t>
+  </si>
+  <si>
+    <t>TI_3.2.1</t>
+  </si>
+  <si>
+    <t>TC_3.2.2</t>
+  </si>
+  <si>
+    <t>TI_3.2.2</t>
+  </si>
+  <si>
+    <t>TC_3.2.3</t>
+  </si>
+  <si>
+    <t>TI_3.2.3</t>
+  </si>
+  <si>
     <t>Data Iterazione: 16/01/2024</t>
-  </si>
-  <si>
-    <t>Test Case ID</t>
-  </si>
-  <si>
-    <t>Test Inciden ID</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Esito</t>
-  </si>
-  <si>
-    <t>Motivo del Warning</t>
-  </si>
-  <si>
-    <t>Test Passati</t>
-  </si>
-  <si>
-    <t>Test non passati</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>TC_1.1_1</t>
-  </si>
-  <si>
-    <t>TI_1.1_1</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>TC_1.1_2</t>
-  </si>
-  <si>
-    <t>TI_1.1_2</t>
-  </si>
-  <si>
-    <t>TC_1.1_3</t>
-  </si>
-  <si>
-    <t>TI_1.1_3</t>
-  </si>
-  <si>
-    <t>Esecuzione accetta</t>
-  </si>
-  <si>
-    <t>TC_1.1_4</t>
-  </si>
-  <si>
-    <t>TI_1.1_4</t>
-  </si>
-  <si>
-    <t>TC_1.1_5</t>
-  </si>
-  <si>
-    <t>TI_1.1_5</t>
-  </si>
-  <si>
-    <t>TC_2.1_1</t>
-  </si>
-  <si>
-    <t>TI_2.1_1</t>
-  </si>
-  <si>
-    <t>TC_2.1_2</t>
-  </si>
-  <si>
-    <t>TI_2.1_2</t>
-  </si>
-  <si>
-    <t>MG</t>
-  </si>
-  <si>
-    <t>TC_2.1_3</t>
-  </si>
-  <si>
-    <t>TI_2.1_3</t>
-  </si>
-  <si>
-    <t>TC_2.1_4</t>
-  </si>
-  <si>
-    <t>TI_2.1_4</t>
-  </si>
-  <si>
-    <t>TC_2.1_5</t>
-  </si>
-  <si>
-    <t>TI_2.1_5</t>
-  </si>
-  <si>
-    <t>TC_2.1_6</t>
-  </si>
-  <si>
-    <t>TI_2.1_6</t>
-  </si>
-  <si>
-    <t>TC_2.1_7</t>
-  </si>
-  <si>
-    <t>TI_2.1_7</t>
-  </si>
-  <si>
-    <t>TC_2.1_8</t>
-  </si>
-  <si>
-    <t>TI_2.1_8</t>
-  </si>
-  <si>
-    <t>TC_2.1_9</t>
-  </si>
-  <si>
-    <t>TI_2.1_9</t>
-  </si>
-  <si>
-    <t>GS</t>
-  </si>
-  <si>
-    <t>TC_2.1_10</t>
-  </si>
-  <si>
-    <t>TI_2.1_10</t>
-  </si>
-  <si>
-    <t>TC_2.1_11</t>
-  </si>
-  <si>
-    <t>TI_2.1_11</t>
-  </si>
-  <si>
-    <t>TC_2.1_12</t>
-  </si>
-  <si>
-    <t>TI_2.1_12</t>
-  </si>
-  <si>
-    <t>TC_2.1_13</t>
-  </si>
-  <si>
-    <t>TI_2.1_13</t>
-  </si>
-  <si>
-    <t>TC_2.1_14</t>
-  </si>
-  <si>
-    <t>TI_2.1_14</t>
-  </si>
-  <si>
-    <t>TC_3.1_1</t>
-  </si>
-  <si>
-    <t>TI_3.1_1</t>
-  </si>
-  <si>
-    <t>TC_3.2_1</t>
-  </si>
-  <si>
-    <t>TI_3.2_1</t>
-  </si>
-  <si>
-    <t>FC</t>
-  </si>
-  <si>
-    <t>TC_3.2_2</t>
-  </si>
-  <si>
-    <t>TI_3.2_2</t>
-  </si>
-  <si>
-    <t>TC_3.2_3</t>
-  </si>
-  <si>
-    <t>TI_3.2_3</t>
-  </si>
-  <si>
-    <t>TC_3.2_4</t>
-  </si>
-  <si>
-    <t>TI_3.2_4</t>
-  </si>
-  <si>
-    <t>TC_3.2_5</t>
-  </si>
-  <si>
-    <t>TI_3.2_5</t>
-  </si>
-  <si>
-    <t>TC_3.2_6</t>
-  </si>
-  <si>
-    <t>TI_3.2_6</t>
-  </si>
-  <si>
-    <t>TC_3.2_7</t>
-  </si>
-  <si>
-    <t>TI_3.2_7</t>
-  </si>
-  <si>
-    <t>IF</t>
-  </si>
-  <si>
-    <t>TC_3.3_1</t>
-  </si>
-  <si>
-    <t>TI_3.3_1</t>
-  </si>
-  <si>
-    <t>TC_3.3_2</t>
-  </si>
-  <si>
-    <t>TI_3.3_2</t>
-  </si>
-  <si>
-    <t>TC_3.3_3</t>
-  </si>
-  <si>
-    <t>TI_3.3_3</t>
-  </si>
-  <si>
-    <t>TC_3.3_4</t>
-  </si>
-  <si>
-    <t>TI_3.3_4</t>
-  </si>
-  <si>
-    <t>TC_3.4_1</t>
-  </si>
-  <si>
-    <t>TI_3.4_1</t>
-  </si>
-  <si>
-    <t>TC_3.4_2</t>
-  </si>
-  <si>
-    <t>TI_3.4_2</t>
-  </si>
-  <si>
-    <t>CE</t>
-  </si>
-  <si>
-    <t>TC_3.4_3</t>
-  </si>
-  <si>
-    <t>TI_3.4_3</t>
-  </si>
-  <si>
-    <t>TC_3.4_4</t>
-  </si>
-  <si>
-    <t>TI_3.4_4</t>
-  </si>
-  <si>
-    <t>TC_3.4_5</t>
-  </si>
-  <si>
-    <t>TI_3.4_5</t>
-  </si>
-  <si>
-    <t>Data Iterazione: 17/01/2024</t>
   </si>
   <si>
     <t>Lista dei team members</t>
@@ -398,7 +527,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,8 +572,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,6 +610,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -501,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -548,6 +695,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -892,14 +1054,14 @@
       <alignment vertical="center" indent="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" indent="0"/>
+      <alignment horizontal="center" vertical="center" indent="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" indent="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment vertical="center" indent="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" indent="0"/>
@@ -992,11 +1154,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabella15" displayName="Tabella15" ref="A2:F38" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A2:F38" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabella15" displayName="Tabella15" ref="A2:F58" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A2:F58" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Test Case ID" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test Inciden ID" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test Incident ID" dataDxfId="28"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Tester" dataDxfId="27"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Data" dataDxfId="26"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Esito" dataDxfId="25"/>
@@ -1011,10 +1173,10 @@
   <autoFilter ref="H2:J3" xr:uid="{D041F23F-50DB-44F5-8399-C3234B0511EE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0F77251A-D071-48D2-B707-A0D5E812CCEF}" name="Test Passati" dataDxfId="21">
-      <calculatedColumnFormula>COUNTIF(E3:E38, "Passed")</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(E3:E58, "Passed")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{6C6E4F92-A1E5-440A-A538-F731811DD1D0}" name="Test non passati" dataDxfId="20">
-      <calculatedColumnFormula>COUNTIF(E3:E38, "Not Passed")</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(E3:E58, "Not Passed")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{F38FF9EA-7BFF-4EA0-BC07-601331118C89}" name="Note" dataDxfId="19"/>
   </tableColumns>
@@ -1027,10 +1189,10 @@
   <autoFilter ref="H2:J3" xr:uid="{D912F910-9C1C-459E-A1F8-589831BC7EE5}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{523D2FA1-2B1A-417F-BBE7-E4726D0B237E}" name="Test Passati" dataDxfId="16">
-      <calculatedColumnFormula>COUNTIF(E3:E38, "Passed")</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(E3:E58, "Passed")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{420B1A33-ADF1-4D47-A9C9-D8CE9FBAD8D0}" name="Test non passati" dataDxfId="15">
-      <calculatedColumnFormula>COUNTIF(E3:E38, "Not Passed")</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(E3:E58, "Not Passed")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{CEF4C0EF-4EDD-4AE0-B380-066173553828}" name="Note" dataDxfId="14"/>
   </tableColumns>
@@ -1039,11 +1201,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C75C6DED-EA6A-47BE-8B8D-1B64C316FA0D}" name="Tabella154" displayName="Tabella154" ref="A2:F38" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A2:F38" xr:uid="{C75C6DED-EA6A-47BE-8B8D-1B64C316FA0D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C75C6DED-EA6A-47BE-8B8D-1B64C316FA0D}" name="Tabella154" displayName="Tabella154" ref="A2:F58" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A2:F58" xr:uid="{C75C6DED-EA6A-47BE-8B8D-1B64C316FA0D}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{97C3CECD-C358-4D41-B58D-345160205BC0}" name="Test Case ID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{5D582B9E-DAFA-4381-A431-093A0769C2C4}" name="Test Inciden ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{5D582B9E-DAFA-4381-A431-093A0769C2C4}" name="Test Incident ID" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{7021FFC5-F98A-4073-96BB-15FF292EC738}" name="Tester" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{A418247A-7583-43B7-B93C-9F7EBB9FF658}" name="Data" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{33E6A2B7-C65D-4C4A-BF03-F1536C5477D7}" name="Esito" dataDxfId="7"/>
@@ -1365,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1392,10 +1554,10 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:11" ht="20.25" customHeight="1">
@@ -1439,721 +1601,1118 @@
         <v>14</v>
       </c>
       <c r="D3" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E3" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="14">
-        <f>COUNTIF(E3:E38, "Passed")</f>
-        <v>36</v>
+        <f>COUNTIF(E3:E58, "Passed")</f>
+        <v>18</v>
       </c>
       <c r="I3" s="14">
-        <f>COUNTIF(E3:E38, "Not Passed")</f>
-        <v>0</v>
+        <f>COUNTIF(E3:E58, "Not Passed")</f>
+        <v>38</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3"/>
     </row>
     <row r="4" spans="1:11" ht="20.25" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E4" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K4"/>
     </row>
     <row r="5" spans="1:11" ht="20.25" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E5" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="H5" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="20.25" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E6" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K6"/>
     </row>
     <row r="7" spans="1:11" ht="20.25" customHeight="1">
       <c r="A7" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K7"/>
     </row>
     <row r="8" spans="1:11" ht="20.25" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E8" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K8"/>
     </row>
     <row r="9" spans="1:11" ht="20.25" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E9" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K9"/>
     </row>
     <row r="10" spans="1:11" ht="20.25" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D10" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E10" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K10"/>
     </row>
     <row r="11" spans="1:11" ht="20.25" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E11" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K11"/>
     </row>
     <row r="12" spans="1:11" ht="20.25" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E12" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K12"/>
     </row>
     <row r="13" spans="1:11" ht="20.25" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E13" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K13"/>
     </row>
     <row r="14" spans="1:11" ht="20.25" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D14" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E14" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K14"/>
     </row>
     <row r="15" spans="1:11" ht="20.25" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E15" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E15" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K15"/>
     </row>
     <row r="16" spans="1:11" ht="20.25" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D16" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E16" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K16"/>
     </row>
     <row r="17" spans="1:11" ht="20.25" customHeight="1">
       <c r="A17" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D17" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E17" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K17"/>
     </row>
     <row r="18" spans="1:11" ht="20.25" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D18" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E18" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="20.25" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D19" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E19" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K19"/>
     </row>
     <row r="20" spans="1:11" ht="20.25" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D20" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E20" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K20"/>
     </row>
     <row r="21" spans="1:11" ht="20.25" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D21" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K21"/>
     </row>
     <row r="22" spans="1:11" ht="20.25" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D22" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K22"/>
     </row>
     <row r="23" spans="1:11" ht="20.25" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D23" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K23"/>
     </row>
     <row r="24" spans="1:11" ht="20.25" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D24" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K24"/>
     </row>
     <row r="25" spans="1:11" ht="20.25" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D25" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K25"/>
     </row>
     <row r="26" spans="1:11" ht="20.25" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D26" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K26"/>
     </row>
     <row r="27" spans="1:11" ht="20.25" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D27" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K27"/>
     </row>
     <row r="28" spans="1:11" ht="20.25" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D28" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K28"/>
     </row>
     <row r="29" spans="1:11" ht="20.25" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D29" s="4">
-        <v>45309</v>
+        <v>45306</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>26</v>
+      </c>
       <c r="K29"/>
     </row>
     <row r="30" spans="1:11" ht="20.25" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B30" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="D30" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E30" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K30"/>
     </row>
     <row r="31" spans="1:11" ht="20.25" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D31" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E31" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E31" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K31"/>
     </row>
     <row r="32" spans="1:11" ht="20.25" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D32" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E32" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K32"/>
     </row>
     <row r="33" spans="1:11" ht="20.25" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D33" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>45306</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="K33"/>
     </row>
     <row r="34" spans="1:11" ht="20.25" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D34" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E34" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K34"/>
     </row>
     <row r="35" spans="1:11" ht="20.25" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D35" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E35" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K35"/>
     </row>
     <row r="36" spans="1:11" ht="20.25" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B36" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="D36" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E36" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E36" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K36"/>
     </row>
     <row r="37" spans="1:11" ht="20.25" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D37" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E37" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E37" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K37"/>
     </row>
     <row r="38" spans="1:11" ht="20.25" customHeight="1">
       <c r="A38" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D38" s="4">
-        <v>45309</v>
-      </c>
-      <c r="E38" s="5" t="s">
+        <v>45306</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A39" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A40" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="K38"/>
-    </row>
-    <row r="39" spans="1:11" ht="20.25" customHeight="1">
-      <c r="K39"/>
-    </row>
-    <row r="40" spans="1:11" ht="20.25" customHeight="1">
+      <c r="F40" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="K40"/>
     </row>
-    <row r="41" spans="1:11" ht="20.25" customHeight="1"/>
-    <row r="42" spans="1:11" ht="20.25" customHeight="1"/>
-    <row r="43" spans="1:11" ht="20.25" customHeight="1"/>
-    <row r="44" spans="1:11" ht="20.25" customHeight="1"/>
-    <row r="45" spans="1:11" ht="20.25" customHeight="1"/>
-    <row r="46" spans="1:11" ht="20.25" customHeight="1"/>
-    <row r="47" spans="1:11" ht="20.25" customHeight="1"/>
-    <row r="48" spans="1:11" ht="20.25" customHeight="1"/>
-    <row r="49" ht="20.25" customHeight="1"/>
-    <row r="50" ht="20.25" customHeight="1"/>
-    <row r="51" ht="20.25" customHeight="1"/>
-    <row r="52" ht="20.25" customHeight="1"/>
-    <row r="53" ht="20.25" customHeight="1"/>
-    <row r="54" ht="20.25" customHeight="1"/>
-    <row r="55" ht="20.25" customHeight="1"/>
-    <row r="56" ht="20.25" customHeight="1"/>
-    <row r="57" ht="20.25" customHeight="1"/>
-    <row r="58" ht="20.25" customHeight="1"/>
-    <row r="59" ht="20.25" customHeight="1"/>
-    <row r="60" ht="20.25" customHeight="1"/>
-    <row r="61" ht="20.25" customHeight="1"/>
-    <row r="62" ht="20.25" customHeight="1"/>
-    <row r="63" ht="20.25" customHeight="1"/>
-    <row r="64" ht="20.25" customHeight="1"/>
+    <row r="41" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A41" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A42" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A43" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A44" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A45" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A46" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A47" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A48" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A49" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A50" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A51" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A52" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A53" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A54" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A55" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A56" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A57" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="4">
+        <v>45306</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="60" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="61" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="62" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="63" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="64" spans="1:6" ht="20.25" customHeight="1"/>
     <row r="65" ht="20.25" customHeight="1"/>
     <row r="66" ht="20.25" customHeight="1"/>
     <row r="67" ht="20.25" customHeight="1"/>
@@ -2171,7 +2730,7 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E38" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E58" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Passed, Not Passed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2186,10 +2745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69355ED8-FCA7-413A-BAEA-157AE9F4A53E}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2213,10 +2772,10 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="18"/>
+      <c r="D1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="23"/>
       <c r="F1" s="16"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2262,37 +2821,37 @@
         <v>14</v>
       </c>
       <c r="D3" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1"/>
       <c r="H3" s="14">
-        <f>COUNTIF(E3:E38, "Passed")</f>
-        <v>36</v>
+        <f>COUNTIF(E3:E58, "Passed")</f>
+        <v>56</v>
       </c>
       <c r="I3" s="14">
-        <f>COUNTIF(E3:E38, "Not Passed")</f>
+        <f>COUNTIF(E3:E58, "Not Passed")</f>
         <v>0</v>
       </c>
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
@@ -2301,42 +2860,42 @@
     </row>
     <row r="5" spans="1:10" ht="15.75">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1"/>
       <c r="H5" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
       <c r="A6" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
@@ -2345,19 +2904,19 @@
     </row>
     <row r="7" spans="1:10" ht="15.75">
       <c r="A7" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1"/>
       <c r="H7" s="1"/>
@@ -2366,19 +2925,19 @@
     </row>
     <row r="8" spans="1:10" ht="15.75">
       <c r="A8" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1"/>
       <c r="H8" s="1"/>
@@ -2387,19 +2946,19 @@
     </row>
     <row r="9" spans="1:10" ht="15.75">
       <c r="A9" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1"/>
       <c r="H9" s="1"/>
@@ -2408,19 +2967,19 @@
     </row>
     <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D10" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F10" s="1"/>
       <c r="H10" s="1"/>
@@ -2429,19 +2988,19 @@
     </row>
     <row r="11" spans="1:10" ht="15.75">
       <c r="A11" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F11" s="1"/>
       <c r="H11" s="1"/>
@@ -2450,19 +3009,19 @@
     </row>
     <row r="12" spans="1:10" ht="15.75">
       <c r="A12" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F12" s="1"/>
       <c r="H12" s="1"/>
@@ -2471,19 +3030,19 @@
     </row>
     <row r="13" spans="1:10" ht="15.75">
       <c r="A13" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F13" s="1"/>
       <c r="H13" s="1"/>
@@ -2492,19 +3051,19 @@
     </row>
     <row r="14" spans="1:10" ht="15.75">
       <c r="A14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D14" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1"/>
       <c r="H14" s="1"/>
@@ -2513,19 +3072,19 @@
     </row>
     <row r="15" spans="1:10" ht="15.75">
       <c r="A15" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F15" s="1"/>
       <c r="H15" s="1"/>
@@ -2534,19 +3093,19 @@
     </row>
     <row r="16" spans="1:10" ht="15.75">
       <c r="A16" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D16" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1"/>
       <c r="H16" s="1"/>
@@ -2555,19 +3114,19 @@
     </row>
     <row r="17" spans="1:10" ht="15.75">
       <c r="A17" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D17" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1"/>
       <c r="H17" s="1"/>
@@ -2576,19 +3135,19 @@
     </row>
     <row r="18" spans="1:10" ht="15.75">
       <c r="A18" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D18" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1"/>
       <c r="H18" s="1"/>
@@ -2597,19 +3156,19 @@
     </row>
     <row r="19" spans="1:10" ht="15.75">
       <c r="A19" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D19" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F19" s="1"/>
       <c r="H19" s="1"/>
@@ -2618,19 +3177,19 @@
     </row>
     <row r="20" spans="1:10" ht="15.75">
       <c r="A20" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D20" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F20" s="1"/>
       <c r="H20" s="1"/>
@@ -2639,19 +3198,19 @@
     </row>
     <row r="21" spans="1:10" ht="15.75">
       <c r="A21" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D21" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F21" s="1"/>
       <c r="H21" s="1"/>
@@ -2660,19 +3219,19 @@
     </row>
     <row r="22" spans="1:10" ht="15.75">
       <c r="A22" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D22" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
@@ -2681,19 +3240,19 @@
     </row>
     <row r="23" spans="1:10" ht="15.75">
       <c r="A23" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D23" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F23" s="1"/>
       <c r="H23" s="1"/>
@@ -2702,19 +3261,19 @@
     </row>
     <row r="24" spans="1:10" ht="15.75">
       <c r="A24" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D24" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F24" s="1"/>
       <c r="H24" s="1"/>
@@ -2723,19 +3282,19 @@
     </row>
     <row r="25" spans="1:10" ht="15.75">
       <c r="A25" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D25" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F25" s="1"/>
       <c r="H25" s="1"/>
@@ -2744,19 +3303,19 @@
     </row>
     <row r="26" spans="1:10" ht="15.75">
       <c r="A26" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D26" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F26" s="1"/>
       <c r="H26" s="1"/>
@@ -2765,19 +3324,19 @@
     </row>
     <row r="27" spans="1:10" ht="15.75">
       <c r="A27" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D27" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F27" s="1"/>
       <c r="H27" s="1"/>
@@ -2786,19 +3345,19 @@
     </row>
     <row r="28" spans="1:10" ht="15.75">
       <c r="A28" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D28" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F28" s="1"/>
       <c r="H28" s="1"/>
@@ -2807,19 +3366,19 @@
     </row>
     <row r="29" spans="1:10" ht="15.75">
       <c r="A29" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D29" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F29" s="1"/>
       <c r="H29" s="1"/>
@@ -2828,19 +3387,19 @@
     </row>
     <row r="30" spans="1:10" ht="15.75">
       <c r="A30" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B30" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="D30" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F30" s="1"/>
       <c r="H30" s="1"/>
@@ -2849,19 +3408,19 @@
     </row>
     <row r="31" spans="1:10" ht="15.75">
       <c r="A31" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D31" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F31" s="1"/>
       <c r="H31" s="1"/>
@@ -2870,19 +3429,19 @@
     </row>
     <row r="32" spans="1:10" ht="15.75">
       <c r="A32" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D32" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F32" s="1"/>
       <c r="H32" s="1"/>
@@ -2891,19 +3450,19 @@
     </row>
     <row r="33" spans="1:10" ht="15.75">
       <c r="A33" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D33" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F33" s="1"/>
       <c r="H33" s="1"/>
@@ -2912,19 +3471,19 @@
     </row>
     <row r="34" spans="1:10" ht="15.75">
       <c r="A34" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D34" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F34" s="1"/>
       <c r="H34" s="1"/>
@@ -2933,19 +3492,19 @@
     </row>
     <row r="35" spans="1:10" ht="15.75">
       <c r="A35" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D35" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F35" s="1"/>
       <c r="H35" s="1"/>
@@ -2954,19 +3513,19 @@
     </row>
     <row r="36" spans="1:10" ht="15.75">
       <c r="A36" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B36" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="D36" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F36" s="1"/>
       <c r="H36" s="1"/>
@@ -2975,19 +3534,19 @@
     </row>
     <row r="37" spans="1:10" ht="15.75">
       <c r="A37" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D37" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F37" s="1"/>
       <c r="H37" s="1"/>
@@ -2996,41 +3555,397 @@
     </row>
     <row r="38" spans="1:10" ht="15.75">
       <c r="A38" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D38" s="4">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" ht="15.75">
+      <c r="A39" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="5"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" ht="15.75">
+      <c r="A40" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="5"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75">
+      <c r="A41" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75">
+      <c r="A42" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75">
+      <c r="A43" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75">
+      <c r="A44" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75">
+      <c r="A45" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75">
+      <c r="A46" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75">
+      <c r="A47" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75">
+      <c r="A48" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75">
+      <c r="A49" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75">
+      <c r="A50" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75">
+      <c r="A51" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75">
+      <c r="A52" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75">
+      <c r="A53" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75">
+      <c r="A54" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75">
+      <c r="A55" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75">
+      <c r="A56" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75">
+      <c r="A57" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75">
+      <c r="A58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="4">
+        <v>45307</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E38" xr:uid="{8D994C4D-9DF1-45AF-872E-577997829556}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E58" xr:uid="{8D994C4D-9DF1-45AF-872E-577997829556}">
       <formula1>"Passed, Not Passed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3060,133 +3975,133 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="15" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>